<commit_message>
finish the card drop of magicbook
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/CardPieceRace.xlsx
+++ b/ConfigData/Xlsx/CardPieceRace.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fish\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="CardPieceRace" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -55,6 +55,26 @@
   </si>
   <si>
     <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropStarMin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropStarMax</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小掉落星级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大掉落星级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -730,74 +750,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -810,12 +762,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:D63" totalsRowShown="0">
-  <autoFilter ref="A1:D63"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:F63" totalsRowShown="0">
+  <autoFilter ref="A1:F63"/>
+  <tableColumns count="6">
     <tableColumn id="4" name="Id"/>
     <tableColumn id="1" name="Rid"/>
     <tableColumn id="2" name="Level"/>
+    <tableColumn id="5" name="DropStarMin"/>
+    <tableColumn id="6" name="DropStarMax"/>
     <tableColumn id="3" name="ItemId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -830,7 +784,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1109,19 +1063,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52:E63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1132,10 +1086,16 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1146,10 +1106,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1160,10 +1126,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>ROW()-3</f>
         <v>1</v>
@@ -1175,10 +1147,16 @@
         <v>1</v>
       </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
         <v>22019001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A63" si="0">ROW()-3</f>
         <v>2</v>
@@ -1190,10 +1168,16 @@
         <v>3</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
         <v>22019002</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1205,10 +1189,16 @@
         <v>5</v>
       </c>
       <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
         <v>22019003</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1220,10 +1210,16 @@
         <v>7</v>
       </c>
       <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
         <v>22019004</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1235,10 +1231,16 @@
         <v>1</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
         <v>22019011</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1250,10 +1252,16 @@
         <v>3</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
         <v>22019012</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1265,10 +1273,16 @@
         <v>5</v>
       </c>
       <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
         <v>22019013</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1280,10 +1294,16 @@
         <v>7</v>
       </c>
       <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
         <v>22019014</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1295,10 +1315,16 @@
         <v>1</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
         <v>22019021</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1310,10 +1336,16 @@
         <v>3</v>
       </c>
       <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
         <v>22019022</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1325,10 +1357,16 @@
         <v>5</v>
       </c>
       <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
         <v>22019023</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1340,10 +1378,16 @@
         <v>7</v>
       </c>
       <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
         <v>22019024</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1355,10 +1399,16 @@
         <v>1</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
         <v>22019031</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1370,10 +1420,16 @@
         <v>3</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
         <v>22019032</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1385,10 +1441,16 @@
         <v>5</v>
       </c>
       <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
         <v>22019033</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1400,10 +1462,16 @@
         <v>7</v>
       </c>
       <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
         <v>22019034</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1415,10 +1483,16 @@
         <v>1</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
         <v>22019041</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1430,10 +1504,16 @@
         <v>3</v>
       </c>
       <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
         <v>22019042</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1445,10 +1525,16 @@
         <v>5</v>
       </c>
       <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
         <v>22019043</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1460,10 +1546,16 @@
         <v>7</v>
       </c>
       <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
         <v>22019044</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1475,10 +1567,16 @@
         <v>1</v>
       </c>
       <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
         <v>22019051</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1490,10 +1588,16 @@
         <v>3</v>
       </c>
       <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
         <v>22019052</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1505,10 +1609,16 @@
         <v>5</v>
       </c>
       <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
         <v>22019053</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1520,10 +1630,16 @@
         <v>7</v>
       </c>
       <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
         <v>22019054</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1535,10 +1651,16 @@
         <v>1</v>
       </c>
       <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
         <v>22019061</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1550,10 +1672,16 @@
         <v>3</v>
       </c>
       <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
         <v>22019062</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1565,10 +1693,16 @@
         <v>5</v>
       </c>
       <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
         <v>22019063</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1580,10 +1714,16 @@
         <v>7</v>
       </c>
       <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
         <v>22019064</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1595,10 +1735,16 @@
         <v>1</v>
       </c>
       <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
         <v>22019071</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1610,10 +1756,16 @@
         <v>3</v>
       </c>
       <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
         <v>22019072</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1625,10 +1777,16 @@
         <v>5</v>
       </c>
       <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
         <v>22019073</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1640,10 +1798,16 @@
         <v>7</v>
       </c>
       <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
         <v>22019074</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1655,10 +1819,16 @@
         <v>1</v>
       </c>
       <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
         <v>22019081</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1670,10 +1840,16 @@
         <v>3</v>
       </c>
       <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
         <v>22019082</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1685,10 +1861,16 @@
         <v>5</v>
       </c>
       <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
         <v>22019083</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1700,10 +1882,16 @@
         <v>7</v>
       </c>
       <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
         <v>22019084</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1715,10 +1903,16 @@
         <v>1</v>
       </c>
       <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
         <v>22019091</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1730,10 +1924,16 @@
         <v>3</v>
       </c>
       <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
         <v>22019092</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1745,10 +1945,16 @@
         <v>5</v>
       </c>
       <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
         <v>22019093</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1760,10 +1966,16 @@
         <v>7</v>
       </c>
       <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43">
         <v>22019094</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1775,10 +1987,16 @@
         <v>1</v>
       </c>
       <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
         <v>22019101</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1790,10 +2008,16 @@
         <v>3</v>
       </c>
       <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
         <v>22019102</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1805,10 +2029,16 @@
         <v>5</v>
       </c>
       <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>7</v>
+      </c>
+      <c r="F46">
         <v>22019103</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1820,10 +2050,16 @@
         <v>7</v>
       </c>
       <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>10</v>
+      </c>
+      <c r="F47">
         <v>22019104</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1835,10 +2071,16 @@
         <v>1</v>
       </c>
       <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
         <v>22019111</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1850,10 +2092,16 @@
         <v>3</v>
       </c>
       <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
         <v>22019112</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1865,10 +2113,16 @@
         <v>5</v>
       </c>
       <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
+      <c r="F50">
         <v>22019113</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1880,10 +2134,16 @@
         <v>7</v>
       </c>
       <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+      <c r="F51">
         <v>22019114</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1895,10 +2155,16 @@
         <v>1</v>
       </c>
       <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
         <v>22019121</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1910,10 +2176,16 @@
         <v>3</v>
       </c>
       <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
         <v>22019122</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1925,10 +2197,16 @@
         <v>5</v>
       </c>
       <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>7</v>
+      </c>
+      <c r="F54">
         <v>22019123</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1940,10 +2218,16 @@
         <v>7</v>
       </c>
       <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55">
         <v>22019124</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1955,10 +2239,16 @@
         <v>1</v>
       </c>
       <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56">
         <v>22019131</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1970,10 +2260,16 @@
         <v>3</v>
       </c>
       <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
         <v>22019132</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1985,10 +2281,16 @@
         <v>5</v>
       </c>
       <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>7</v>
+      </c>
+      <c r="F58">
         <v>22019133</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2000,10 +2302,16 @@
         <v>7</v>
       </c>
       <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>10</v>
+      </c>
+      <c r="F59">
         <v>22019134</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2015,10 +2323,16 @@
         <v>1</v>
       </c>
       <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>4</v>
+      </c>
+      <c r="F60">
         <v>22019141</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2030,10 +2344,16 @@
         <v>3</v>
       </c>
       <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>5</v>
+      </c>
+      <c r="F61">
         <v>22019142</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2045,10 +2365,16 @@
         <v>5</v>
       </c>
       <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62">
         <v>22019143</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2060,6 +2386,12 @@
         <v>7</v>
       </c>
       <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63">
+        <v>10</v>
+      </c>
+      <c r="F63">
         <v>22019144</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rearange the code of random item manage.
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/CardPieceRace.xlsx
+++ b/ConfigData/Xlsx/CardPieceRace.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +241,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +434,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,11 +688,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,8 +746,84 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -739,10 +836,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F90" totalsRowShown="0">
-  <autoFilter ref="A3:F90"/>
-  <sortState ref="A4:F90">
-    <sortCondition ref="A3:A90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F88" totalsRowShown="0">
+  <autoFilter ref="A3:F88"/>
+  <sortState ref="A4:F84">
+    <sortCondition ref="A3:A84"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Id"/>
@@ -764,7 +861,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1043,34 +1140,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79:F90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1115,7 +1213,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>22018001</v>
       </c>
       <c r="B4">
@@ -1135,7 +1233,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>22018002</v>
       </c>
       <c r="B5">
@@ -1155,7 +1253,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>22018003</v>
       </c>
       <c r="B6">
@@ -1175,7 +1273,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>22018011</v>
       </c>
       <c r="B7">
@@ -1195,7 +1293,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>22018012</v>
       </c>
       <c r="B8">
@@ -1215,7 +1313,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>22018013</v>
       </c>
       <c r="B9">
@@ -1235,7 +1333,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>22018021</v>
       </c>
       <c r="B10">
@@ -1255,7 +1353,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>22018022</v>
       </c>
       <c r="B11">
@@ -1275,7 +1373,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>22018023</v>
       </c>
       <c r="B12">
@@ -1295,7 +1393,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>22018031</v>
       </c>
       <c r="B13">
@@ -1315,7 +1413,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>22018032</v>
       </c>
       <c r="B14">
@@ -1335,7 +1433,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>22018033</v>
       </c>
       <c r="B15">
@@ -1355,7 +1453,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>22018041</v>
       </c>
       <c r="B16">
@@ -1375,7 +1473,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>22018042</v>
       </c>
       <c r="B17">
@@ -1395,7 +1493,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>22018043</v>
       </c>
       <c r="B18">
@@ -1415,7 +1513,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>22018051</v>
       </c>
       <c r="B19">
@@ -1435,7 +1533,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>22018052</v>
       </c>
       <c r="B20">
@@ -1455,7 +1553,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>22018053</v>
       </c>
       <c r="B21">
@@ -1475,7 +1573,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>22018061</v>
       </c>
       <c r="B22">
@@ -1495,7 +1593,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>22018062</v>
       </c>
       <c r="B23">
@@ -1515,7 +1613,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>22018063</v>
       </c>
       <c r="B24">
@@ -1536,1321 +1634,1281 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>22018071</v>
+        <v>22019011</v>
       </c>
       <c r="B25">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>22018072</v>
+        <v>22019012</v>
       </c>
       <c r="B26">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>22018073</v>
+        <v>22019013</v>
       </c>
       <c r="B27">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>22018081</v>
+        <v>22019014</v>
       </c>
       <c r="B28">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>22018082</v>
+        <v>22019021</v>
       </c>
       <c r="B29">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>22018083</v>
+        <v>22019022</v>
       </c>
       <c r="B30">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>22019001</v>
+        <v>22019023</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>-1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>22019002</v>
+        <v>22019024</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32">
         <v>-1</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F32">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>22019003</v>
+        <v>22019031</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>22019004</v>
+        <v>22019032</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>22019011</v>
+        <v>22019033</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>-1</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>22019012</v>
+        <v>22019034</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F36">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>22019013</v>
+        <v>22019041</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>22019014</v>
+        <v>22019042</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E38">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F38">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>22019021</v>
+        <v>22019043</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>22019022</v>
+        <v>22019044</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>-1</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>22019023</v>
+        <v>22019051</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>-1</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>22019024</v>
+        <v>22019052</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>-1</v>
       </c>
       <c r="D42">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E42">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F42">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>22019031</v>
+        <v>22019053</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>22019032</v>
+        <v>22019054</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>-1</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F44">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>22019033</v>
+        <v>22019061</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C45">
         <v>-1</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>22019034</v>
+        <v>22019062</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C46">
         <v>-1</v>
       </c>
       <c r="D46">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E46">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F46">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>22019041</v>
+        <v>22019063</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C47">
         <v>-1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>22019042</v>
+        <v>22019064</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C48">
         <v>-1</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F48">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49">
-        <v>22019043</v>
+        <v>22019071</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C49">
         <v>-1</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50">
-        <v>22019044</v>
+        <v>22019072</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C50">
         <v>-1</v>
       </c>
       <c r="D50">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E50">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F50">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51">
-        <v>22019051</v>
+        <v>22019073</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>-1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52">
-        <v>22019052</v>
+        <v>22019074</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F52">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53">
-        <v>22019053</v>
+        <v>22019081</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C53">
         <v>-1</v>
       </c>
       <c r="D53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54">
-        <v>22019054</v>
+        <v>22019082</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C54">
         <v>-1</v>
       </c>
       <c r="D54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F54">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55">
-        <v>22019061</v>
+        <v>22019083</v>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <v>-1</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F55">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56">
-        <v>22019062</v>
+        <v>22019084</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <v>-1</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E56">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F56">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57">
-        <v>22019063</v>
+        <v>22019091</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C57">
         <v>-1</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>22019064</v>
+        <v>22019092</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C58">
         <v>-1</v>
       </c>
       <c r="D58">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E58">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F58">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>22019071</v>
+        <v>22019093</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>-1</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F59">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>22019072</v>
+        <v>22019094</v>
       </c>
       <c r="B60">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C60">
         <v>-1</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F60">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61">
-        <v>22019073</v>
+        <v>22019101</v>
       </c>
       <c r="B61">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C61">
         <v>-1</v>
       </c>
       <c r="D61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F61">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62">
-        <v>22019074</v>
+        <v>22019102</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C62">
         <v>-1</v>
       </c>
       <c r="D62">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E62">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F62">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63">
-        <v>22019081</v>
+        <v>22019103</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C63">
         <v>-1</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F63">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64">
-        <v>22019082</v>
+        <v>22019104</v>
       </c>
       <c r="B64">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C64">
         <v>-1</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F64">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65">
-        <v>22019083</v>
+        <v>22019111</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C65">
         <v>-1</v>
       </c>
       <c r="D65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F65">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66">
-        <v>22019084</v>
+        <v>22019112</v>
       </c>
       <c r="B66">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C66">
         <v>-1</v>
       </c>
       <c r="D66">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E66">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F66">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67">
-        <v>22019091</v>
+        <v>22019113</v>
       </c>
       <c r="B67">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C67">
         <v>-1</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68">
-        <v>22019092</v>
+        <v>22019114</v>
       </c>
       <c r="B68">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C68">
         <v>-1</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E68">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F68">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69">
-        <v>22019093</v>
+        <v>22019121</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C69">
         <v>-1</v>
       </c>
       <c r="D69">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F69">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70">
-        <v>22019094</v>
+        <v>22019122</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C70">
         <v>-1</v>
       </c>
       <c r="D70">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E70">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F70">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71">
-        <v>22019101</v>
+        <v>22019123</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C71">
         <v>-1</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F71">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72">
-        <v>22019102</v>
+        <v>22019124</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <v>-1</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F72">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73">
-        <v>22019103</v>
+        <v>22019131</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C73">
         <v>-1</v>
       </c>
       <c r="D73">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E73">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F73">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74">
-        <v>22019104</v>
+        <v>22019132</v>
       </c>
       <c r="B74">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C74">
         <v>-1</v>
       </c>
       <c r="D74">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E74">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F74">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75">
-        <v>22019111</v>
+        <v>22019133</v>
       </c>
       <c r="B75">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C75">
         <v>-1</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76">
-        <v>22019112</v>
+        <v>22019134</v>
       </c>
       <c r="B76">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C76">
         <v>-1</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E76">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F76">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77">
-        <v>22019113</v>
+        <v>22019141</v>
       </c>
       <c r="B77">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C77">
         <v>-1</v>
       </c>
       <c r="D77">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F77">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78">
-        <v>22019114</v>
+        <v>22019142</v>
       </c>
       <c r="B78">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C78">
         <v>-1</v>
       </c>
       <c r="D78">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E78">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F78">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79">
-        <v>22019121</v>
+        <v>22019143</v>
       </c>
       <c r="B79">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C79">
         <v>-1</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F79">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80">
-        <v>22019122</v>
+        <v>22019144</v>
       </c>
       <c r="B80">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C80">
         <v>-1</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E80">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F80">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22019123</v>
+        <v>22019151</v>
       </c>
       <c r="B81">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C81">
         <v>-1</v>
       </c>
       <c r="D81">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F81">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82">
-        <v>22019124</v>
+        <v>22019152</v>
       </c>
       <c r="B82">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C82">
         <v>-1</v>
       </c>
       <c r="D82">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E82">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F82">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83">
-        <v>22019131</v>
+        <v>22019153</v>
       </c>
       <c r="B83">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C83">
         <v>-1</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F83">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84">
-        <v>22019132</v>
+        <v>22019154</v>
       </c>
       <c r="B84">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C84">
         <v>-1</v>
       </c>
       <c r="D84">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E84">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F84">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85">
-        <v>22019133</v>
+        <v>22019161</v>
       </c>
       <c r="B85">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C85">
         <v>-1</v>
       </c>
       <c r="D85">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F85">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86">
-        <v>22019134</v>
+        <v>22019162</v>
       </c>
       <c r="B86">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C86">
         <v>-1</v>
       </c>
       <c r="D86">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E86">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F86">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87">
-        <v>22019141</v>
+        <v>22019163</v>
       </c>
       <c r="B87">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C87">
         <v>-1</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F87">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88">
-        <v>22019142</v>
+        <v>22019164</v>
       </c>
       <c r="B88">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C88">
         <v>-1</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F88">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89">
-        <v>22019143</v>
-      </c>
-      <c r="B89">
-        <v>14</v>
-      </c>
-      <c r="C89">
-        <v>-1</v>
-      </c>
-      <c r="D89">
-        <v>5</v>
-      </c>
-      <c r="E89">
-        <v>5</v>
-      </c>
-      <c r="F89">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A90">
-        <v>22019144</v>
-      </c>
-      <c r="B90">
-        <v>14</v>
-      </c>
-      <c r="C90">
-        <v>-1</v>
-      </c>
-      <c r="D90">
-        <v>7</v>
-      </c>
-      <c r="E90">
-        <v>7</v>
-      </c>
-      <c r="F90">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
genelize the price of items
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/CardPieceRace.xlsx
+++ b/ConfigData/Xlsx/CardPieceRace.xlsx
@@ -746,15 +746,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -836,8 +828,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F88" totalsRowShown="0">
-  <autoFilter ref="A3:F88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F95" totalsRowShown="0">
+  <autoFilter ref="A3:F95"/>
   <sortState ref="A4:F84">
     <sortCondition ref="A3:A84"/>
   </sortState>
@@ -1140,16 +1132,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.75" customWidth="1"/>
+    <col min="2" max="6" width="6.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1223,13 +1215,13 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1243,13 +1235,13 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1263,38 +1255,38 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>22018011</v>
+        <v>22018004</v>
       </c>
       <c r="B7">
         <v>-1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>22018012</v>
+        <v>22018011</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -1303,18 +1295,18 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>22018013</v>
+        <v>22018012</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -1323,58 +1315,58 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <v>22018021</v>
+        <v>22018013</v>
       </c>
       <c r="B10">
         <v>-1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <v>22018022</v>
+        <v>22018014</v>
       </c>
       <c r="B11">
         <v>-1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <v>22018023</v>
+        <v>22018021</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -1383,30 +1375,30 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>22018031</v>
+        <v>22018022</v>
       </c>
       <c r="B13">
         <v>-1</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -1414,13 +1406,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <v>22018032</v>
+        <v>22018023</v>
       </c>
       <c r="B14">
         <v>-1</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1434,13 +1426,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <v>22018033</v>
+        <v>22018024</v>
       </c>
       <c r="B15">
         <v>-1</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -1454,1447 +1446,1447 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <v>22018041</v>
+        <v>22018031</v>
       </c>
       <c r="B16">
         <v>-1</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <v>22018042</v>
+        <v>22018032</v>
       </c>
       <c r="B17">
         <v>-1</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <v>22018043</v>
+        <v>22018033</v>
       </c>
       <c r="B18">
         <v>-1</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <v>22018051</v>
+        <v>22018034</v>
       </c>
       <c r="B19">
         <v>-1</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
-        <v>22018052</v>
+        <v>22018041</v>
       </c>
       <c r="B20">
         <v>-1</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
-        <v>22018053</v>
+        <v>22018042</v>
       </c>
       <c r="B21">
         <v>-1</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
-        <v>22018061</v>
+        <v>22018043</v>
       </c>
       <c r="B22">
         <v>-1</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
-        <v>22018062</v>
+        <v>22018044</v>
       </c>
       <c r="B23">
         <v>-1</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
+        <v>22018051</v>
+      </c>
+      <c r="B24">
+        <v>-1</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>22018052</v>
+      </c>
+      <c r="B25">
+        <v>-1</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>22018053</v>
+      </c>
+      <c r="B26">
+        <v>-1</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>22018054</v>
+      </c>
+      <c r="B27">
+        <v>-1</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>22018061</v>
+      </c>
+      <c r="B28">
+        <v>-1</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>22018062</v>
+      </c>
+      <c r="B29">
+        <v>-1</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
         <v>22018063</v>
       </c>
-      <c r="B24">
-        <v>-1</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24">
-        <v>6</v>
-      </c>
-      <c r="F24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25">
-        <v>22019011</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>-1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>22019012</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>-1</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
-      </c>
-      <c r="F26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>22019013</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>-1</v>
-      </c>
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27">
-        <v>5</v>
-      </c>
-      <c r="F27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>22019014</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>-1</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29">
-        <v>22019021</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <v>-1</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>22019022</v>
-      </c>
       <c r="B30">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31">
-        <v>22019023</v>
+      <c r="A31" s="2">
+        <v>22018064</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C31">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>22019024</v>
+        <v>22019011</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>-1</v>
       </c>
       <c r="D32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>22019031</v>
+        <v>22019012</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>22019032</v>
+        <v>22019013</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>22019033</v>
+        <v>22019014</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>-1</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F35">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>22019034</v>
+        <v>22019021</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>22019041</v>
+        <v>22019022</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>22019042</v>
+        <v>22019023</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F38">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>22019043</v>
+        <v>22019024</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F39">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>22019044</v>
+        <v>22019031</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>-1</v>
       </c>
       <c r="D40">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>22019051</v>
+        <v>22019032</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>-1</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>22019052</v>
+        <v>22019033</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>-1</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F42">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>22019053</v>
+        <v>22019034</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F43">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>22019054</v>
+        <v>22019041</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>-1</v>
       </c>
       <c r="D44">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F44">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>22019061</v>
+        <v>22019042</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>-1</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>22019062</v>
+        <v>22019043</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>-1</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>22019063</v>
+        <v>22019044</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>-1</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F47">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>22019064</v>
+        <v>22019051</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>-1</v>
       </c>
       <c r="D48">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F48">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49">
-        <v>22019071</v>
+        <v>22019052</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>-1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50">
-        <v>22019072</v>
+        <v>22019053</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>-1</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F50">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51">
-        <v>22019073</v>
+        <v>22019054</v>
       </c>
       <c r="B51">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>-1</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F51">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52">
-        <v>22019074</v>
+        <v>22019061</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F52">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53">
-        <v>22019081</v>
+        <v>22019062</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <v>-1</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54">
-        <v>22019082</v>
+        <v>22019063</v>
       </c>
       <c r="B54">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C54">
         <v>-1</v>
       </c>
       <c r="D54">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F54">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55">
-        <v>22019083</v>
+        <v>22019064</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>-1</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E55">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F55">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56">
-        <v>22019084</v>
+        <v>22019071</v>
       </c>
       <c r="B56">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56">
         <v>-1</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F56">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57">
-        <v>22019091</v>
+        <v>22019072</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C57">
         <v>-1</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>22019092</v>
+        <v>22019073</v>
       </c>
       <c r="B58">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C58">
         <v>-1</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F58">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>22019093</v>
+        <v>22019074</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C59">
         <v>-1</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E59">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F59">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>22019094</v>
+        <v>22019081</v>
       </c>
       <c r="B60">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60">
         <v>-1</v>
       </c>
       <c r="D60">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F60">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61">
-        <v>22019101</v>
+        <v>22019082</v>
       </c>
       <c r="B61">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C61">
         <v>-1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62">
-        <v>22019102</v>
+        <v>22019083</v>
       </c>
       <c r="B62">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C62">
         <v>-1</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F62">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63">
-        <v>22019103</v>
+        <v>22019084</v>
       </c>
       <c r="B63">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C63">
         <v>-1</v>
       </c>
       <c r="D63">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E63">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F63">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64">
-        <v>22019104</v>
+        <v>22019091</v>
       </c>
       <c r="B64">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C64">
         <v>-1</v>
       </c>
       <c r="D64">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F64">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65">
-        <v>22019111</v>
+        <v>22019092</v>
       </c>
       <c r="B65">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C65">
         <v>-1</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F65">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66">
-        <v>22019112</v>
+        <v>22019093</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C66">
         <v>-1</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E66">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F66">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67">
-        <v>22019113</v>
+        <v>22019094</v>
       </c>
       <c r="B67">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C67">
         <v>-1</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E67">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F67">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68">
-        <v>22019114</v>
+        <v>22019101</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C68">
         <v>-1</v>
       </c>
       <c r="D68">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F68">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69">
-        <v>22019121</v>
+        <v>22019102</v>
       </c>
       <c r="B69">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C69">
         <v>-1</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70">
-        <v>22019122</v>
+        <v>22019103</v>
       </c>
       <c r="B70">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C70">
         <v>-1</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E70">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F70">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71">
-        <v>22019123</v>
+        <v>22019104</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C71">
         <v>-1</v>
       </c>
       <c r="D71">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E71">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F71">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72">
-        <v>22019124</v>
+        <v>22019111</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C72">
         <v>-1</v>
       </c>
       <c r="D72">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E72">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F72">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73">
-        <v>22019131</v>
+        <v>22019112</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C73">
         <v>-1</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F73">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74">
-        <v>22019132</v>
+        <v>22019113</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C74">
         <v>-1</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F74">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75">
-        <v>22019133</v>
+        <v>22019114</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C75">
         <v>-1</v>
       </c>
       <c r="D75">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E75">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F75">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76">
-        <v>22019134</v>
+        <v>22019121</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C76">
         <v>-1</v>
       </c>
       <c r="D76">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E76">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F76">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77">
-        <v>22019141</v>
+        <v>22019122</v>
       </c>
       <c r="B77">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C77">
         <v>-1</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F77">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78">
-        <v>22019142</v>
+        <v>22019123</v>
       </c>
       <c r="B78">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C78">
         <v>-1</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E78">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F78">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79">
-        <v>22019143</v>
+        <v>22019124</v>
       </c>
       <c r="B79">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C79">
         <v>-1</v>
       </c>
       <c r="D79">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F79">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80">
-        <v>22019144</v>
+        <v>22019131</v>
       </c>
       <c r="B80">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C80">
         <v>-1</v>
       </c>
       <c r="D80">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F80">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22019151</v>
+        <v>22019132</v>
       </c>
       <c r="B81">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C81">
         <v>-1</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F81">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82">
-        <v>22019152</v>
+        <v>22019133</v>
       </c>
       <c r="B82">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C82">
         <v>-1</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E82">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F82">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83">
-        <v>22019153</v>
+        <v>22019134</v>
       </c>
       <c r="B83">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C83">
         <v>-1</v>
       </c>
       <c r="D83">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E83">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F83">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84">
-        <v>22019154</v>
+        <v>22019141</v>
       </c>
       <c r="B84">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C84">
         <v>-1</v>
       </c>
       <c r="D84">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F84">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85">
-        <v>22019161</v>
+        <v>22019142</v>
       </c>
       <c r="B85">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C85">
         <v>-1</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F85">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86">
-        <v>22019162</v>
+        <v>22019143</v>
       </c>
       <c r="B86">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C86">
         <v>-1</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E86">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F86">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87">
-        <v>22019163</v>
+        <v>22019144</v>
       </c>
       <c r="B87">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C87">
         <v>-1</v>
       </c>
       <c r="D87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F87">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88">
-        <v>22019164</v>
+        <v>22019151</v>
       </c>
       <c r="B88">
         <v>15</v>
@@ -2903,12 +2895,152 @@
         <v>-1</v>
       </c>
       <c r="D88">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>22019152</v>
+      </c>
+      <c r="B89">
+        <v>15</v>
+      </c>
+      <c r="C89">
+        <v>-1</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89">
+        <v>3</v>
+      </c>
+      <c r="F89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>22019153</v>
+      </c>
+      <c r="B90">
+        <v>15</v>
+      </c>
+      <c r="C90">
+        <v>-1</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>22019154</v>
+      </c>
+      <c r="B91">
+        <v>15</v>
+      </c>
+      <c r="C91">
+        <v>-1</v>
+      </c>
+      <c r="D91">
+        <v>7</v>
+      </c>
+      <c r="E91">
+        <v>7</v>
+      </c>
+      <c r="F91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>22019161</v>
+      </c>
+      <c r="B92">
+        <v>15</v>
+      </c>
+      <c r="C92">
+        <v>-1</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>22019162</v>
+      </c>
+      <c r="B93">
+        <v>15</v>
+      </c>
+      <c r="C93">
+        <v>-1</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="F93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>22019163</v>
+      </c>
+      <c r="B94">
+        <v>15</v>
+      </c>
+      <c r="C94">
+        <v>-1</v>
+      </c>
+      <c r="D94">
+        <v>5</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+      <c r="F94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>22019164</v>
+      </c>
+      <c r="B95">
+        <v>15</v>
+      </c>
+      <c r="C95">
+        <v>-1</v>
+      </c>
+      <c r="D95">
+        <v>7</v>
+      </c>
+      <c r="E95">
+        <v>7</v>
+      </c>
+      <c r="F95">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rearange the ids of items
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/CardPieceRace.xlsx
+++ b/ConfigData/Xlsx/CardPieceRace.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,12 +434,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,14 +682,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -748,74 +739,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -846,14 +769,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -921,6 +844,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -956,6 +896,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1145,22 +1102,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1205,8 +1162,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
-        <v>22018001</v>
+      <c r="A4">
+        <v>22101001</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -1225,8 +1182,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
-        <v>22018002</v>
+      <c r="A5">
+        <v>22101002</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -1245,8 +1202,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
-        <v>22018003</v>
+      <c r="A6">
+        <v>22101003</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -1265,8 +1222,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
-        <v>22018004</v>
+      <c r="A7">
+        <v>22101004</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -1285,8 +1242,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
-        <v>22018011</v>
+      <c r="A8">
+        <v>22101011</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -1305,8 +1262,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
-        <v>22018012</v>
+      <c r="A9">
+        <v>22101012</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -1325,8 +1282,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
-        <v>22018013</v>
+      <c r="A10">
+        <v>22101013</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -1345,8 +1302,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
-        <v>22018014</v>
+      <c r="A11">
+        <v>22101014</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -1365,8 +1322,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
-        <v>22018021</v>
+      <c r="A12">
+        <v>22101021</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -1385,8 +1342,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
-        <v>22018022</v>
+      <c r="A13">
+        <v>22101022</v>
       </c>
       <c r="B13">
         <v>-1</v>
@@ -1405,8 +1362,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
-        <v>22018023</v>
+      <c r="A14">
+        <v>22101023</v>
       </c>
       <c r="B14">
         <v>-1</v>
@@ -1425,8 +1382,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
-        <v>22018024</v>
+      <c r="A15">
+        <v>22101024</v>
       </c>
       <c r="B15">
         <v>-1</v>
@@ -1445,8 +1402,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
-        <v>22018031</v>
+      <c r="A16">
+        <v>22101031</v>
       </c>
       <c r="B16">
         <v>-1</v>
@@ -1465,8 +1422,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
-        <v>22018032</v>
+      <c r="A17">
+        <v>22101032</v>
       </c>
       <c r="B17">
         <v>-1</v>
@@ -1485,8 +1442,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
-        <v>22018033</v>
+      <c r="A18">
+        <v>22101033</v>
       </c>
       <c r="B18">
         <v>-1</v>
@@ -1505,8 +1462,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
-        <v>22018034</v>
+      <c r="A19">
+        <v>22101034</v>
       </c>
       <c r="B19">
         <v>-1</v>
@@ -1525,8 +1482,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
-        <v>22018041</v>
+      <c r="A20">
+        <v>22101041</v>
       </c>
       <c r="B20">
         <v>-1</v>
@@ -1545,8 +1502,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
-        <v>22018042</v>
+      <c r="A21">
+        <v>22101042</v>
       </c>
       <c r="B21">
         <v>-1</v>
@@ -1565,8 +1522,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
-        <v>22018043</v>
+      <c r="A22">
+        <v>22101043</v>
       </c>
       <c r="B22">
         <v>-1</v>
@@ -1585,8 +1542,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
-        <v>22018044</v>
+      <c r="A23">
+        <v>22101044</v>
       </c>
       <c r="B23">
         <v>-1</v>
@@ -1605,8 +1562,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
-        <v>22018051</v>
+      <c r="A24">
+        <v>22101051</v>
       </c>
       <c r="B24">
         <v>-1</v>
@@ -1625,8 +1582,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="2">
-        <v>22018052</v>
+      <c r="A25">
+        <v>22101052</v>
       </c>
       <c r="B25">
         <v>-1</v>
@@ -1645,8 +1602,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="2">
-        <v>22018053</v>
+      <c r="A26">
+        <v>22101053</v>
       </c>
       <c r="B26">
         <v>-1</v>
@@ -1665,8 +1622,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="2">
-        <v>22018054</v>
+      <c r="A27">
+        <v>22101054</v>
       </c>
       <c r="B27">
         <v>-1</v>
@@ -1685,8 +1642,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
-        <v>22018061</v>
+      <c r="A28">
+        <v>22101061</v>
       </c>
       <c r="B28">
         <v>-1</v>
@@ -1705,8 +1662,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="2">
-        <v>22018062</v>
+      <c r="A29">
+        <v>22101062</v>
       </c>
       <c r="B29">
         <v>-1</v>
@@ -1725,8 +1682,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="2">
-        <v>22018063</v>
+      <c r="A30">
+        <v>22101063</v>
       </c>
       <c r="B30">
         <v>-1</v>
@@ -1745,8 +1702,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="2">
-        <v>22018064</v>
+      <c r="A31">
+        <v>22101064</v>
       </c>
       <c r="B31">
         <v>-1</v>
@@ -1766,7 +1723,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>22019011</v>
+        <v>22102011</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1786,7 +1743,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>22019012</v>
+        <v>22102012</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1806,7 +1763,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>22019013</v>
+        <v>22102013</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1826,7 +1783,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>22019014</v>
+        <v>22102014</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1846,7 +1803,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>22019021</v>
+        <v>22102021</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1866,7 +1823,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>22019022</v>
+        <v>22102022</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -1886,7 +1843,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>22019023</v>
+        <v>22102023</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -1906,7 +1863,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>22019024</v>
+        <v>22102024</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1926,7 +1883,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>22019031</v>
+        <v>22102031</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1946,7 +1903,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>22019032</v>
+        <v>22102032</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -1966,7 +1923,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>22019033</v>
+        <v>22102033</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1986,7 +1943,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>22019034</v>
+        <v>22102034</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -2006,7 +1963,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>22019041</v>
+        <v>22102041</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -2026,7 +1983,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>22019042</v>
+        <v>22102042</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -2046,7 +2003,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>22019043</v>
+        <v>22102043</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -2066,7 +2023,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>22019044</v>
+        <v>22102044</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -2086,7 +2043,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>22019051</v>
+        <v>22102051</v>
       </c>
       <c r="B48">
         <v>5</v>
@@ -2106,7 +2063,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49">
-        <v>22019052</v>
+        <v>22102052</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -2126,7 +2083,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50">
-        <v>22019053</v>
+        <v>22102053</v>
       </c>
       <c r="B50">
         <v>5</v>
@@ -2146,7 +2103,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51">
-        <v>22019054</v>
+        <v>22102054</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -2166,7 +2123,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52">
-        <v>22019061</v>
+        <v>22102061</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -2186,7 +2143,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53">
-        <v>22019062</v>
+        <v>22102062</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -2206,7 +2163,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54">
-        <v>22019063</v>
+        <v>22102063</v>
       </c>
       <c r="B54">
         <v>6</v>
@@ -2226,7 +2183,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55">
-        <v>22019064</v>
+        <v>22102064</v>
       </c>
       <c r="B55">
         <v>6</v>
@@ -2246,7 +2203,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56">
-        <v>22019071</v>
+        <v>22102071</v>
       </c>
       <c r="B56">
         <v>7</v>
@@ -2266,7 +2223,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57">
-        <v>22019072</v>
+        <v>22102072</v>
       </c>
       <c r="B57">
         <v>7</v>
@@ -2286,7 +2243,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>22019073</v>
+        <v>22102073</v>
       </c>
       <c r="B58">
         <v>7</v>
@@ -2306,7 +2263,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>22019074</v>
+        <v>22102074</v>
       </c>
       <c r="B59">
         <v>7</v>
@@ -2326,7 +2283,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>22019081</v>
+        <v>22102081</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -2346,7 +2303,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61">
-        <v>22019082</v>
+        <v>22102082</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -2366,7 +2323,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62">
-        <v>22019083</v>
+        <v>22102083</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -2386,7 +2343,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63">
-        <v>22019084</v>
+        <v>22102084</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -2406,7 +2363,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64">
-        <v>22019091</v>
+        <v>22102091</v>
       </c>
       <c r="B64">
         <v>9</v>
@@ -2426,7 +2383,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65">
-        <v>22019092</v>
+        <v>22102092</v>
       </c>
       <c r="B65">
         <v>9</v>
@@ -2446,7 +2403,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66">
-        <v>22019093</v>
+        <v>22102093</v>
       </c>
       <c r="B66">
         <v>9</v>
@@ -2466,7 +2423,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67">
-        <v>22019094</v>
+        <v>22102094</v>
       </c>
       <c r="B67">
         <v>9</v>
@@ -2486,7 +2443,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68">
-        <v>22019101</v>
+        <v>22102101</v>
       </c>
       <c r="B68">
         <v>10</v>
@@ -2506,7 +2463,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69">
-        <v>22019102</v>
+        <v>22102102</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -2526,7 +2483,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70">
-        <v>22019103</v>
+        <v>22102103</v>
       </c>
       <c r="B70">
         <v>10</v>
@@ -2546,7 +2503,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71">
-        <v>22019104</v>
+        <v>22102104</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -2566,7 +2523,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72">
-        <v>22019111</v>
+        <v>22102111</v>
       </c>
       <c r="B72">
         <v>11</v>
@@ -2586,7 +2543,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73">
-        <v>22019112</v>
+        <v>22102112</v>
       </c>
       <c r="B73">
         <v>11</v>
@@ -2606,7 +2563,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74">
-        <v>22019113</v>
+        <v>22102113</v>
       </c>
       <c r="B74">
         <v>11</v>
@@ -2626,7 +2583,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75">
-        <v>22019114</v>
+        <v>22102114</v>
       </c>
       <c r="B75">
         <v>11</v>
@@ -2646,7 +2603,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76">
-        <v>22019121</v>
+        <v>22102121</v>
       </c>
       <c r="B76">
         <v>12</v>
@@ -2666,7 +2623,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77">
-        <v>22019122</v>
+        <v>22102122</v>
       </c>
       <c r="B77">
         <v>12</v>
@@ -2686,7 +2643,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78">
-        <v>22019123</v>
+        <v>22102123</v>
       </c>
       <c r="B78">
         <v>12</v>
@@ -2706,7 +2663,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79">
-        <v>22019124</v>
+        <v>22102124</v>
       </c>
       <c r="B79">
         <v>12</v>
@@ -2726,7 +2683,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80">
-        <v>22019131</v>
+        <v>22102131</v>
       </c>
       <c r="B80">
         <v>13</v>
@@ -2746,7 +2703,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22019132</v>
+        <v>22102132</v>
       </c>
       <c r="B81">
         <v>13</v>
@@ -2766,7 +2723,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82">
-        <v>22019133</v>
+        <v>22102133</v>
       </c>
       <c r="B82">
         <v>13</v>
@@ -2786,7 +2743,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83">
-        <v>22019134</v>
+        <v>22102134</v>
       </c>
       <c r="B83">
         <v>13</v>
@@ -2806,7 +2763,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84">
-        <v>22019141</v>
+        <v>22102141</v>
       </c>
       <c r="B84">
         <v>14</v>
@@ -2826,7 +2783,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85">
-        <v>22019142</v>
+        <v>22102142</v>
       </c>
       <c r="B85">
         <v>14</v>
@@ -2846,7 +2803,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86">
-        <v>22019143</v>
+        <v>22102143</v>
       </c>
       <c r="B86">
         <v>14</v>
@@ -2866,7 +2823,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87">
-        <v>22019144</v>
+        <v>22102144</v>
       </c>
       <c r="B87">
         <v>14</v>
@@ -2886,7 +2843,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88">
-        <v>22019151</v>
+        <v>22102151</v>
       </c>
       <c r="B88">
         <v>15</v>
@@ -2906,7 +2863,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89">
-        <v>22019152</v>
+        <v>22102152</v>
       </c>
       <c r="B89">
         <v>15</v>
@@ -2926,7 +2883,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90">
-        <v>22019153</v>
+        <v>22102153</v>
       </c>
       <c r="B90">
         <v>15</v>
@@ -2946,7 +2903,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91">
-        <v>22019154</v>
+        <v>22102154</v>
       </c>
       <c r="B91">
         <v>15</v>
@@ -2966,7 +2923,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92">
-        <v>22019161</v>
+        <v>22102161</v>
       </c>
       <c r="B92">
         <v>15</v>
@@ -2986,7 +2943,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93">
-        <v>22019162</v>
+        <v>22102162</v>
       </c>
       <c r="B93">
         <v>15</v>
@@ -3006,7 +2963,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94">
-        <v>22019163</v>
+        <v>22102163</v>
       </c>
       <c r="B94">
         <v>15</v>
@@ -3026,7 +2983,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95">
-        <v>22019164</v>
+        <v>22102164</v>
       </c>
       <c r="B95">
         <v>15</v>

</xml_diff>